<commit_message>
some waypoints for enemy wave patterns
</commit_message>
<xml_diff>
--- a/_docs/tables.xlsx
+++ b/_docs/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>player</t>
   </si>
@@ -34,6 +34,48 @@
   </si>
   <si>
     <t>send</t>
+  </si>
+  <si>
+    <t>top left</t>
+  </si>
+  <si>
+    <t>top right</t>
+  </si>
+  <si>
+    <t>bot left</t>
+  </si>
+  <si>
+    <t>bot right</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>top cent</t>
+  </si>
+  <si>
+    <t>orig</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>transform storage</t>
+  </si>
+  <si>
+    <t>LB diag</t>
+  </si>
+  <si>
+    <t>RB diag</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -63,7 +105,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,8 +122,14 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -104,17 +152,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -418,20 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -445,7 +516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -457,7 +528,7 @@
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -466,7 +537,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -475,7 +546,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -483,6 +554,173 @@
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
       <c r="F6" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>-5</v>
+      </c>
+      <c r="C9">
+        <v>6.5</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>-3.75</v>
+      </c>
+      <c r="G9">
+        <v>-6.25</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>6.5</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>3.75</v>
+      </c>
+      <c r="G10">
+        <v>-1.75</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>3.75</v>
+      </c>
+      <c r="J10">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>-5</v>
+      </c>
+      <c r="C11">
+        <v>-7.5</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="6">
+        <f>F9+F10</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="6">
+        <f>G9+G10</f>
+        <v>-8</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="6">
+        <f>I10-I9</f>
+        <v>3.75</v>
+      </c>
+      <c r="J11" s="6">
+        <f>J10-J9</f>
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>-7.5</v>
+      </c>
+      <c r="G14">
+        <v>-3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>7.5</v>
+      </c>
+      <c r="G15">
+        <v>-3.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>